<commit_message>
reverted back to full defining snp file
</commit_message>
<xml_diff>
--- a/dependencies/mycobacterium/tbc/af2122/script_dependents/script2/DefiningSNPsGroupDesignations.xlsx
+++ b/dependencies/mycobacterium/tbc/af2122/script_dependents/script2/DefiningSNPsGroupDesignations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/snp_analysis/dependencies/mycobacterium/tbc/af2122/script_dependents/script2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/root/TStuber/Results/mycobacterium/tbc/af2122/script_dependents/script2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AAB78922-BC93-C84E-8DDA-08012A9E5F99}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1B1B7DE8-DAD3-8A43-9F85-C73F0F804C9D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="460" windowWidth="25140" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13340" yWindow="580" windowWidth="25140" windowHeight="27300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,996 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="330">
+  <si>
+    <t>Mbovis-01</t>
+  </si>
+  <si>
+    <t>Mbovis-02</t>
+  </si>
+  <si>
+    <t>Mbovis-03</t>
+  </si>
+  <si>
+    <t>Mbovis-04</t>
+  </si>
+  <si>
+    <t>Mbovis-05</t>
+  </si>
+  <si>
+    <t>Mbovis-06</t>
+  </si>
+  <si>
+    <t>Mbovis-07</t>
+  </si>
+  <si>
+    <t>Mbovis-08</t>
+  </si>
+  <si>
+    <t>Mbovis-09</t>
+  </si>
+  <si>
+    <t>Mbovis-10</t>
+  </si>
+  <si>
+    <t>Mbovis-11</t>
+  </si>
+  <si>
+    <t>Mbovis-12</t>
+  </si>
+  <si>
+    <t>Mbovis-13</t>
+  </si>
+  <si>
+    <t>Mbovis-14</t>
+  </si>
+  <si>
+    <t>Mbovis-15</t>
+  </si>
+  <si>
+    <t>Mbovis-16</t>
+  </si>
+  <si>
+    <t>Mbovis-17</t>
+  </si>
+  <si>
+    <t>Mbovis-18</t>
+  </si>
+  <si>
+    <t>Mbovis-19</t>
+  </si>
+  <si>
+    <t>Mbovis-20</t>
+  </si>
+  <si>
+    <t>Mbovis-21</t>
+  </si>
+  <si>
+    <t>Mbovis-22</t>
+  </si>
+  <si>
+    <t>Mbovis-23</t>
+  </si>
+  <si>
+    <t>Mbovis-24</t>
+  </si>
+  <si>
+    <t>Mbovis-25</t>
+  </si>
+  <si>
+    <t>Mbovis-26</t>
+  </si>
+  <si>
+    <t>Mbovis-28</t>
+  </si>
+  <si>
+    <t>Mbovis-29</t>
+  </si>
+  <si>
+    <t>Mbovis-30</t>
+  </si>
+  <si>
+    <t>Mbovis-31</t>
+  </si>
+  <si>
+    <t>Mbovis-32</t>
+  </si>
+  <si>
+    <t>Mbovis-33</t>
+  </si>
+  <si>
+    <t>Mbovis-34</t>
+  </si>
+  <si>
+    <t>Mbovis-TB</t>
+  </si>
+  <si>
+    <t>Mbovis-01A</t>
+  </si>
+  <si>
+    <t>Mbovis-01A1</t>
+  </si>
+  <si>
+    <t>Mbovis-01A2</t>
+  </si>
+  <si>
+    <t>Mbovis-01A3</t>
+  </si>
+  <si>
+    <t>Mbovis-01A4</t>
+  </si>
+  <si>
+    <t>Mbovis-01A5</t>
+  </si>
+  <si>
+    <t>Mbovis-01B</t>
+  </si>
+  <si>
+    <t>Mbovis-01B1</t>
+  </si>
+  <si>
+    <t>Mbovis-01B2</t>
+  </si>
+  <si>
+    <t>Mbovis-01C</t>
+  </si>
+  <si>
+    <t>Mbovis-01C1</t>
+  </si>
+  <si>
+    <t>Mbovis-01C2</t>
+  </si>
+  <si>
+    <t>Mbovis-01D</t>
+  </si>
+  <si>
+    <t>Mbovis-01D1</t>
+  </si>
+  <si>
+    <t>Mbovis-01D2</t>
+  </si>
+  <si>
+    <t>Mbovis-01D3</t>
+  </si>
+  <si>
+    <t>Mbovis-01D4</t>
+  </si>
+  <si>
+    <t>Mbovis-01D5</t>
+  </si>
+  <si>
+    <t>Mbovis-01D6</t>
+  </si>
+  <si>
+    <t>Mbovis-01D7</t>
+  </si>
+  <si>
+    <t>Mbovis-02A</t>
+  </si>
+  <si>
+    <t>Mbovis-02B</t>
+  </si>
+  <si>
+    <t>Mbovis-02C</t>
+  </si>
+  <si>
+    <t>Mbovis-04A</t>
+  </si>
+  <si>
+    <t>Mbovis-04B</t>
+  </si>
+  <si>
+    <t>Mbovis-04B1</t>
+  </si>
+  <si>
+    <t>Mbovis-04B2</t>
+  </si>
+  <si>
+    <t>Mbovis-04B3</t>
+  </si>
+  <si>
+    <t>Mbovis-04B4</t>
+  </si>
+  <si>
+    <t>Mbovis-04B5</t>
+  </si>
+  <si>
+    <t>Mbovis-04B6</t>
+  </si>
   <si>
     <t>Mbovis-04B7</t>
   </si>
   <si>
+    <t>Mbovis-04C</t>
+  </si>
+  <si>
+    <t>Mbovis-05A</t>
+  </si>
+  <si>
+    <t>Mbovis-05B</t>
+  </si>
+  <si>
+    <t>Mbovis-06A</t>
+  </si>
+  <si>
+    <t>Mbovis-06B</t>
+  </si>
+  <si>
+    <t>Mbovis-07A</t>
+  </si>
+  <si>
+    <t>Mbovis-07B</t>
+  </si>
+  <si>
+    <t>Mbovis-07B1</t>
+  </si>
+  <si>
+    <t>Mbovis-07B2</t>
+  </si>
+  <si>
+    <t>Mbovis-07B3</t>
+  </si>
+  <si>
+    <t>Mbovis-14A</t>
+  </si>
+  <si>
+    <t>Mbovis-14B</t>
+  </si>
+  <si>
+    <t>Mbovis-16A</t>
+  </si>
+  <si>
+    <t>Mbovis-16B</t>
+  </si>
+  <si>
+    <t>Mbovis-16C</t>
+  </si>
+  <si>
+    <t>Mbovis-16D</t>
+  </si>
+  <si>
+    <t>Mbovis-16E</t>
+  </si>
+  <si>
+    <t>Mbovis-17A</t>
+  </si>
+  <si>
+    <t>Mbovis-17A1</t>
+  </si>
+  <si>
+    <t>Mbovis-17B</t>
+  </si>
+  <si>
+    <t>Mbovis-17B1</t>
+  </si>
+  <si>
+    <t>Mbovis-17B2</t>
+  </si>
+  <si>
+    <t>Mbovis-17B3</t>
+  </si>
+  <si>
+    <t>Mbovis-17B4</t>
+  </si>
+  <si>
+    <t>Mbovis-17B5</t>
+  </si>
+  <si>
+    <t>Mbovis-17B6</t>
+  </si>
+  <si>
+    <t>Mbovis-17C</t>
+  </si>
+  <si>
+    <t>Mbovis-17D</t>
+  </si>
+  <si>
+    <t>Mbovis-17E</t>
+  </si>
+  <si>
+    <t>Mbovis-17F</t>
+  </si>
+  <si>
+    <t>Mbovis-18A</t>
+  </si>
+  <si>
+    <t>Mbovis-19A</t>
+  </si>
+  <si>
+    <t>Mbovis-19A1</t>
+  </si>
+  <si>
+    <t>Mbovis-19B</t>
+  </si>
+  <si>
+    <t>Mbovis-19C</t>
+  </si>
+  <si>
+    <t>Mbovis-19E</t>
+  </si>
+  <si>
+    <t>Mbovis-21A</t>
+  </si>
+  <si>
+    <t>Mbovis-21B</t>
+  </si>
+  <si>
+    <t>Mbovis-23A</t>
+  </si>
+  <si>
+    <t>Mbovis-23A1</t>
+  </si>
+  <si>
+    <t>Mbovis-23A2</t>
+  </si>
+  <si>
+    <t>Mbovis-23B</t>
+  </si>
+  <si>
+    <t>Mbovis-23B1</t>
+  </si>
+  <si>
+    <t>Mbovis-23C</t>
+  </si>
+  <si>
+    <t>Mbovis-23E</t>
+  </si>
+  <si>
+    <t>Mbovis-29A</t>
+  </si>
+  <si>
     <t>Grouping</t>
   </si>
   <si>
     <t>Absolute position</t>
   </si>
   <si>
+    <t>Mbovis-35</t>
+  </si>
+  <si>
+    <t>Mbovis-36</t>
+  </si>
+  <si>
+    <t>Mbovis-23B2</t>
+  </si>
+  <si>
+    <t>Mbovis-23D</t>
+  </si>
+  <si>
+    <t>Mcaprae-27A</t>
+  </si>
+  <si>
+    <t>Mcaprae-27B</t>
+  </si>
+  <si>
+    <t>Mcaprae-27B1</t>
+  </si>
+  <si>
+    <t>Mcaprae-27B2</t>
+  </si>
+  <si>
+    <t>Mcaprae-27</t>
+  </si>
+  <si>
+    <t>Mbovis-31A</t>
+  </si>
+  <si>
+    <t>Mbovis-31A1</t>
+  </si>
+  <si>
+    <t>Mbovis-31A2</t>
+  </si>
+  <si>
+    <t>Mbovis-31A3</t>
+  </si>
+  <si>
+    <t>Mbovis-31B</t>
+  </si>
+  <si>
+    <t>Mbovis-31C</t>
+  </si>
+  <si>
+    <t>Mbovis-31C1</t>
+  </si>
+  <si>
+    <t>Mbovis-31C2</t>
+  </si>
+  <si>
+    <t>Mbovis-31D</t>
+  </si>
+  <si>
+    <t>NC_002945.4-34863</t>
+  </si>
+  <si>
+    <t>NC_002945.4-177287</t>
+  </si>
+  <si>
+    <t>NC_002945.4-178647</t>
+  </si>
+  <si>
+    <t>NC_002945.4-195737</t>
+  </si>
+  <si>
+    <t>NC_002945.4-237923</t>
+  </si>
+  <si>
+    <t>NC_002945.4-265453</t>
+  </si>
+  <si>
+    <t>NC_002945.4-308852</t>
+  </si>
+  <si>
+    <t>NC_002945.4-389472</t>
+  </si>
+  <si>
+    <t>NC_002945.4-545803</t>
+  </si>
+  <si>
+    <t>NC_002945.4-655025</t>
+  </si>
+  <si>
+    <t>NC_002945.4-748733</t>
+  </si>
+  <si>
+    <t>NC_002945.4-751671</t>
+  </si>
+  <si>
+    <t>NC_002945.4-768011</t>
+  </si>
+  <si>
+    <t>NC_002945.4-779123</t>
+  </si>
+  <si>
+    <t>NC_002945.4-937683</t>
+  </si>
+  <si>
+    <t>NC_002945.4-943203</t>
+  </si>
+  <si>
+    <t>NC_002945.4-952614</t>
+  </si>
+  <si>
+    <t>NC_002945.4-960492</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1030829</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1033229</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1038839</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1048291</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1061663</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1079889</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1082060</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1083373</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1095172</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1129861</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1135324</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1141190</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1141620</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1158639</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1162423</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1179954</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1182407</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1238941</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1254487</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1259431</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1292852</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1295549</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1299369</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1344785</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1361126</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1371487</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1446965</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1462755</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1478045</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1485817</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1499464</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1517653</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1584651</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1612340</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1613129</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1617986</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1622803</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1624515</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1635895</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1668725</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1701236</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1701920</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1790349</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1814064</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1830046</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1848283</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1872263</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1888685</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1924735</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1945505</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1946619</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1950718</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1962242</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1969776</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2005215</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2033870</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2073009</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2095909</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2108312</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2134170</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2138896</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2197617</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2201396</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2216552</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2232592</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2235560</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2322516</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2323696</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2411032</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2468017</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2497409</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2546958</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2589954</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2601169</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2728822</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2778919</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2829139</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2865305</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2884747</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2926459</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2926759</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2928920</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2944962</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2998141</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3032080</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3043696</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3073557</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3150557</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3185411</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3203015</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3209992</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3233531</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3234625</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3260138</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3275732</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3353644</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3364144</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3377064</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3451956</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3523804</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3553753</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3585549</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3633840</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3915086</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3926916</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3930712</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3975860</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3978462</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4022029</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4052766</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4058211</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4142432</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4150894</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4199939</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4219410</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4250477</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4293068</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4345429</t>
+  </si>
+  <si>
+    <t>Mbovis-13A</t>
+  </si>
+  <si>
+    <t>Mbovis-13B</t>
+  </si>
+  <si>
+    <t>Mbovis-13C</t>
+  </si>
+  <si>
+    <t>Mbovis-14B1</t>
+  </si>
+  <si>
+    <t>Mbovis-14B2</t>
+  </si>
+  <si>
+    <t>Mbovis-14B3</t>
+  </si>
+  <si>
+    <t>Mbovis-21ABCG</t>
+  </si>
+  <si>
+    <t>Mbovis-21Awild</t>
+  </si>
+  <si>
+    <t>Morygis</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1402322</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1489088</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1197896</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1233743</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1814262</t>
+  </si>
+  <si>
+    <t>NC_002945.4-139460</t>
+  </si>
+  <si>
+    <t>Mbovis-14B4</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3126504</t>
+  </si>
+  <si>
+    <t>Mbovis-14C</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1915861</t>
+  </si>
+  <si>
+    <t>NC_002945.4-558746</t>
+  </si>
+  <si>
+    <t>Mbovis-13A1</t>
+  </si>
+  <si>
+    <t>Mbovis-13A2</t>
+  </si>
+  <si>
+    <t>Mbovis-13A3</t>
+  </si>
+  <si>
+    <t>NC_002945.4-903153</t>
+  </si>
+  <si>
+    <t>Mbovis-21Awild-1</t>
+  </si>
+  <si>
+    <t>Mbovis-21Awild-2</t>
+  </si>
+  <si>
+    <t>Mbovis-21Awild-3</t>
+  </si>
+  <si>
+    <t>NC_002945.4-164974</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1611238</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4305135</t>
+  </si>
+  <si>
+    <t>Mbovis-11A</t>
+  </si>
+  <si>
+    <t>Mbovis-11B</t>
+  </si>
+  <si>
+    <t>Mbovis-11B-1</t>
+  </si>
+  <si>
+    <t>Mbovis-11B-2</t>
+  </si>
+  <si>
+    <t>NC_002945.4-198388</t>
+  </si>
+  <si>
+    <t>NC_002945.4-3822669</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4310185</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1003896</t>
+  </si>
+  <si>
+    <t>Group_1-5</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2899163</t>
+  </si>
+  <si>
+    <t>NC_002945.4-288778</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1356374</t>
+  </si>
+  <si>
+    <t>Group_10-14</t>
+  </si>
+  <si>
+    <t>Group_9_15</t>
+  </si>
+  <si>
+    <t>NC_002945.4-2145868!</t>
+  </si>
+  <si>
+    <t>hodgepodge</t>
+  </si>
+  <si>
+    <t>NC_002945.4-4060755</t>
+  </si>
+  <si>
+    <t>Mbovis-23C1</t>
+  </si>
+  <si>
+    <t>Mbovis-23C2</t>
+  </si>
+  <si>
+    <t>Mbovis-23C3</t>
+  </si>
+  <si>
+    <t>Mbovis-21B1</t>
+  </si>
+  <si>
+    <t>Mbovis-21B2</t>
+  </si>
+  <si>
+    <t>NC_002945.4-319719</t>
+  </si>
+  <si>
+    <t>NC_002945.4-124271</t>
+  </si>
+  <si>
+    <t>Mbovis-21B3</t>
+  </si>
+  <si>
+    <t>NC_002945.4-699598</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1332559</t>
+  </si>
+  <si>
+    <t>Mbovis-14A1</t>
+  </si>
+  <si>
     <t>NC_002945.4-3468394</t>
+  </si>
+  <si>
+    <t>Mbovis-04B7A</t>
+  </si>
+  <si>
+    <t>Mbovis-04B7B</t>
+  </si>
+  <si>
+    <t>NC_002945.4-1002057</t>
   </si>
 </sst>
 </file>
@@ -76,12 +1054,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -410,7 +1400,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -422,6 +1412,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1018,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,10 +2031,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1044,12 +2042,1324 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>3</v>
       </c>
+      <c r="B28" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>298</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>299</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>300</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>301</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>268</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>288</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>289</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>290</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>269</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>270</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>325</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>271</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>272</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>273</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>283</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>285</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>78</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>97</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>98</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>99</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>19</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>102</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>103</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>318</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>319</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>322</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>21</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>22</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>104</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>105</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>106</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>107</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>108</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>116</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>109</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>315</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>316</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>317</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>117</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>110</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>23</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>24</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>25</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>26</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>27</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>111</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>28</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>29</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>30</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>31</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>32</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>114</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>115</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>33</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>122</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>118</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>119</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>120</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>121</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162"/>
+      <c r="B162"/>
+      <c r="D162" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163"/>
+      <c r="B163"/>
+      <c r="D163" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E163" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164"/>
+      <c r="B164"/>
+      <c r="D164" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E164" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165"/>
+      <c r="B165"/>
+      <c r="D165" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>312</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="D2:E2">
-    <sortCondition ref="D2"/>
+  <sortState ref="D2:E143">
+    <sortCondition ref="D2:D143"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>